<commit_message>
Move files to public/
</commit_message>
<xml_diff>
--- a/src/public/productos-prueba-espejo_v2.xlsx
+++ b/src/public/productos-prueba-espejo_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2E49C7-0776-405F-A742-5FA5EDCCA6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311E93A1-CDF4-4D8F-9ECB-7B4A0E9CF304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="6135" windowWidth="16200" windowHeight="9360" xr2:uid="{5FCE9BD9-161B-4910-8247-CD58469831A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5FCE9BD9-161B-4910-8247-CD58469831A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo Prueba" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Category</t>
   </si>
@@ -190,13 +190,7 @@
     <t>1;1;1</t>
   </si>
   <si>
-    <t>L,M;L,M</t>
-  </si>
-  <si>
-    <t>1,1;1,1</t>
-  </si>
-  <si>
-    <t>20310135,1212121;20310132,1212120</t>
+    <t>20310135;12121212</t>
   </si>
 </sst>
 </file>
@@ -613,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAF92C7-A778-4305-BA92-0305C7282631}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,13 +670,13 @@
         <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>